<commit_message>
LogIn validation. Addition of more words to the hangman data base. Final details, comments and corrections.
</commit_message>
<xml_diff>
--- a/1Homework/DataBase/hangmanWords.xlsx
+++ b/1Homework/DataBase/hangmanWords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollo Web Duodécimo\Programación para web\PRIMER SEMESTRE\1 TAREA\1Homework\1Homework\DataBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Desarrollo Web Duodécimo\Programación para web\PRIMER SEMESTRE\1 TAREA\1Homework\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D796BAE-BD97-4C20-8142-509C76B9D43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F701C06-4BAA-4972-823D-E7BD7AFF6213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Words</t>
   </si>
@@ -58,6 +58,51 @@
   </si>
   <si>
     <t>jukebox</t>
+  </si>
+  <si>
+    <t>xanadu</t>
+  </si>
+  <si>
+    <t>cowabunga</t>
+  </si>
+  <si>
+    <t>wannabe</t>
+  </si>
+  <si>
+    <t>radical</t>
+  </si>
+  <si>
+    <t>cool</t>
+  </si>
+  <si>
+    <t>duh</t>
+  </si>
+  <si>
+    <t>cd</t>
+  </si>
+  <si>
+    <t>nerd</t>
+  </si>
+  <si>
+    <t>dude</t>
+  </si>
+  <si>
+    <t>chill</t>
+  </si>
+  <si>
+    <t>whatever</t>
+  </si>
+  <si>
+    <t>dynamite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gnarly </t>
+  </si>
+  <si>
+    <t>disco</t>
+  </si>
+  <si>
+    <t>groove</t>
   </si>
 </sst>
 </file>
@@ -375,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,50 +443,128 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A26">
+    <sortCondition ref="A26"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>